<commit_message>
xlsx parsing, simple api created, zipcode validation using zippo and xlsx created api
</commit_message>
<xml_diff>
--- a/data/exutilityRateData.xlsx
+++ b/data/exutilityRateData.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adry.walsh\OneDrive\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25317"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12800"/>
   </bookViews>
   <sheets>
     <sheet name="utilityRates" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -200,7 +198,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -293,7 +291,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -345,7 +343,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -539,7 +537,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -547,25 +545,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -588,7 +586,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>43081</v>
       </c>
@@ -611,7 +609,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>43081</v>
       </c>
@@ -634,7 +632,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>43081</v>
       </c>
@@ -657,7 +655,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>43081</v>
       </c>
@@ -680,7 +678,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>43081</v>
       </c>
@@ -703,7 +701,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>43081</v>
       </c>
@@ -726,7 +724,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>43081</v>
       </c>
@@ -749,7 +747,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>43081</v>
       </c>
@@ -772,7 +770,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>43081</v>
       </c>
@@ -795,7 +793,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>43081</v>
       </c>
@@ -818,7 +816,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>43081</v>
       </c>
@@ -841,7 +839,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>43081</v>
       </c>
@@ -864,7 +862,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>43081</v>
       </c>
@@ -887,7 +885,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>43081</v>
       </c>
@@ -910,7 +908,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>43081</v>
       </c>
@@ -933,7 +931,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>43081</v>
       </c>
@@ -956,7 +954,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>43081</v>
       </c>
@@ -979,7 +977,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>43081</v>
       </c>
@@ -1002,7 +1000,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>43081</v>
       </c>
@@ -1025,7 +1023,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>43081</v>
       </c>
@@ -1048,7 +1046,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>43081</v>
       </c>
@@ -1071,7 +1069,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>43081</v>
       </c>
@@ -1094,7 +1092,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>43081</v>
       </c>
@@ -1117,7 +1115,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>43081</v>
       </c>
@@ -1140,7 +1138,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>43081</v>
       </c>
@@ -1163,7 +1161,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>43081</v>
       </c>
@@ -1186,7 +1184,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>43081</v>
       </c>
@@ -1209,7 +1207,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>43081</v>
       </c>
@@ -1232,7 +1230,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>43081</v>
       </c>
@@ -1255,7 +1253,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>43081</v>
       </c>
@@ -1278,7 +1276,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>43081</v>
       </c>
@@ -1301,7 +1299,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="1">
         <v>43081</v>
       </c>
@@ -1324,7 +1322,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="1">
         <v>43081</v>
       </c>
@@ -1347,7 +1345,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="1">
         <v>43081</v>
       </c>
@@ -1370,7 +1368,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="1">
         <v>43081</v>
       </c>
@@ -1393,7 +1391,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="1">
         <v>43081</v>
       </c>
@@ -1416,7 +1414,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="1">
         <v>43081</v>
       </c>
@@ -1439,7 +1437,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="1">
         <v>43081</v>
       </c>
@@ -1462,7 +1460,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="1">
         <v>43081</v>
       </c>
@@ -1485,7 +1483,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="1">
         <v>43081</v>
       </c>
@@ -1513,5 +1511,10 @@
     <sortCondition ref="G2:G41"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refacotring for better maintainability
</commit_message>
<xml_diff>
--- a/data/exutilityRateData.xlsx
+++ b/data/exutilityRateData.xlsx
@@ -537,7 +537,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -548,8 +548,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>